<commit_message>
feat: nieuwe perspectieven bij datapunten (zelfreflectie, docent, student-P, student-HF1, student-HF2/3, stagebegeleider, patiënt, overig) + iconen
</commit_message>
<xml_diff>
--- a/public/Cursus-info/25-26-Cursussen-EVL-thema-kennis.xlsx
+++ b/public/Cursus-info/25-26-Cursussen-EVL-thema-kennis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Jouw Portfolio plan\public\Cursus-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD3A6CC-CAC7-4869-9337-DE25DFAEB3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197F2EA3-0705-463B-8FAE-6AE787F1980D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-60" windowWidth="19420" windowHeight="10300" xr2:uid="{74C3179E-11BE-4A40-B8D0-1805AFCFBDBB}"/>
+    <workbookView xWindow="1128" yWindow="1116" windowWidth="14376" windowHeight="7296" xr2:uid="{74C3179E-11BE-4A40-B8D0-1805AFCFBDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="58">
   <si>
-    <t>Return2Performande</t>
-  </si>
-  <si>
     <t>Fit in the Hood</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Kennis</t>
+  </si>
+  <si>
+    <t>Return2Performance</t>
   </si>
 </sst>
 </file>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82D385D-79E2-4B99-A96C-A1CB23B97714}">
   <dimension ref="A1:AO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AM12" sqref="AM12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,1018 +627,1018 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>54</v>
       </c>
-      <c r="V1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>38</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>40</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>41</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>44</v>
       </c>
-      <c r="AB2" t="s">
-        <v>45</v>
-      </c>
       <c r="AK2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>47</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>48</v>
       </c>
-      <c r="AC3" t="s">
-        <v>49</v>
-      </c>
       <c r="AK3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA4" t="s">
         <v>46</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>47</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>48</v>
       </c>
-      <c r="AC4" t="s">
-        <v>49</v>
-      </c>
       <c r="AK4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA5" t="s">
         <v>46</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>47</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>48</v>
       </c>
-      <c r="AC5" t="s">
-        <v>49</v>
-      </c>
       <c r="AK5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA6" t="s">
         <v>46</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>47</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>48</v>
       </c>
-      <c r="AC6" t="s">
-        <v>49</v>
-      </c>
       <c r="AK6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA7" t="s">
         <v>46</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>47</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>48</v>
       </c>
-      <c r="AC7" t="s">
-        <v>49</v>
-      </c>
       <c r="AK7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA8" t="s">
         <v>46</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>47</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>48</v>
       </c>
-      <c r="AC8" t="s">
-        <v>49</v>
-      </c>
       <c r="AK8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AK9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AO10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>